<commit_message>
[Docs] EPBDS-5036, 5038, 5041, 5150, updated Doc Instruction, added diagram
</commit_message>
<xml_diff>
--- a/Docs/org.openl.tablets.doc/draft/Examples/Corporate Rating_TableParts.xlsx
+++ b/Docs/org.openl.tablets.doc/draft/Examples/Corporate Rating_TableParts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830" tabRatio="860" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830" tabRatio="860" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Rating Algorithm" sheetId="4" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="523">
   <si>
     <t>Domain Model</t>
   </si>
@@ -3789,6 +3789,103 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> column 2 of 2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">SimpleRules DoubleValue </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FinRatioWeight</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (FinancialRatio financialRatio) </t>
+    </r>
+  </si>
+  <si>
+    <t>precision</t>
+  </si>
+  <si>
+    <t>financialRatio</t>
+  </si>
+  <si>
+    <t>_res_ (2)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FinRatioWeight</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> FinRatioWeightTest1 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>FinRatioWeight</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Franklin Gothic Book"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> FinRatioWeightTest2 </t>
     </r>
   </si>
 </sst>
@@ -4261,7 +4358,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4550,17 +4647,14 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4574,17 +4668,29 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4613,12 +4719,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -4627,6 +4727,12 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4646,11 +4752,8 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -5015,12 +5118,12 @@
     </row>
     <row r="6" spans="2:8" ht="105" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="12"/>
-      <c r="C6" s="126" t="s">
+      <c r="C6" s="139" t="s">
         <v>501</v>
       </c>
-      <c r="D6" s="126"/>
-      <c r="E6" s="126"/>
-      <c r="F6" s="126"/>
+      <c r="D6" s="139"/>
+      <c r="E6" s="139"/>
+      <c r="F6" s="139"/>
       <c r="G6" s="12"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
@@ -5033,12 +5136,12 @@
     </row>
     <row r="8" spans="2:8" ht="19.5" x14ac:dyDescent="0.35">
       <c r="B8" s="12"/>
-      <c r="C8" s="129" t="s">
+      <c r="C8" s="135" t="s">
         <v>440</v>
       </c>
-      <c r="D8" s="129"/>
-      <c r="E8" s="129"/>
-      <c r="F8" s="129"/>
+      <c r="D8" s="135"/>
+      <c r="E8" s="135"/>
+      <c r="F8" s="135"/>
       <c r="G8" s="12"/>
     </row>
     <row r="9" spans="2:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -5049,18 +5152,18 @@
       <c r="D9" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="E9" s="130" t="s">
+      <c r="E9" s="129" t="s">
         <v>494</v>
       </c>
-      <c r="F9" s="130"/>
+      <c r="F9" s="129"/>
       <c r="G9" s="12"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="12"/>
-      <c r="C10" s="131" t="s">
+      <c r="C10" s="130" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="131"/>
+      <c r="D10" s="130"/>
       <c r="E10" s="45" t="s">
         <v>65</v>
       </c>
@@ -5071,10 +5174,10 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="12"/>
-      <c r="C11" s="130" t="s">
+      <c r="C11" s="129" t="s">
         <v>379</v>
       </c>
-      <c r="D11" s="130"/>
+      <c r="D11" s="129"/>
       <c r="E11" s="3"/>
       <c r="F11" s="47" t="s">
         <v>124</v>
@@ -5086,10 +5189,10 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="12"/>
-      <c r="C12" s="128" t="s">
+      <c r="C12" s="138" t="s">
         <v>378</v>
       </c>
-      <c r="D12" s="128"/>
+      <c r="D12" s="138"/>
       <c r="E12" s="115"/>
       <c r="F12" s="47" t="s">
         <v>381</v>
@@ -5098,10 +5201,10 @@
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="12"/>
-      <c r="C13" s="128" t="s">
+      <c r="C13" s="138" t="s">
         <v>209</v>
       </c>
-      <c r="D13" s="128"/>
+      <c r="D13" s="138"/>
       <c r="E13" s="115" t="s">
         <v>463</v>
       </c>
@@ -5112,11 +5215,11 @@
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="12"/>
-      <c r="C14" s="128" t="s">
+      <c r="C14" s="138" t="s">
         <v>314</v>
       </c>
-      <c r="D14" s="128"/>
-      <c r="E14" s="127" t="s">
+      <c r="D14" s="138"/>
+      <c r="E14" s="140" t="s">
         <v>488</v>
       </c>
       <c r="F14" s="47" t="s">
@@ -5126,11 +5229,11 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="12"/>
-      <c r="C15" s="128" t="s">
+      <c r="C15" s="138" t="s">
         <v>350</v>
       </c>
-      <c r="D15" s="128"/>
-      <c r="E15" s="127"/>
+      <c r="D15" s="138"/>
+      <c r="E15" s="140"/>
       <c r="F15" s="47" t="s">
         <v>380</v>
       </c>
@@ -5138,11 +5241,11 @@
     </row>
     <row r="16" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="12"/>
-      <c r="C16" s="128" t="s">
+      <c r="C16" s="138" t="s">
         <v>374</v>
       </c>
-      <c r="D16" s="128"/>
-      <c r="E16" s="127"/>
+      <c r="D16" s="138"/>
+      <c r="E16" s="140"/>
       <c r="F16" s="47" t="s">
         <v>383</v>
       </c>
@@ -5150,10 +5253,10 @@
     </row>
     <row r="17" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="12"/>
-      <c r="C17" s="128" t="s">
+      <c r="C17" s="138" t="s">
         <v>416</v>
       </c>
-      <c r="D17" s="128"/>
+      <c r="D17" s="138"/>
       <c r="E17" s="75" t="s">
         <v>489</v>
       </c>
@@ -5167,10 +5270,10 @@
     </row>
     <row r="18" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="12"/>
-      <c r="C18" s="133" t="s">
+      <c r="C18" s="132" t="s">
         <v>392</v>
       </c>
-      <c r="D18" s="133"/>
+      <c r="D18" s="132"/>
       <c r="E18" s="3" t="s">
         <v>464</v>
       </c>
@@ -5184,10 +5287,10 @@
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="12"/>
-      <c r="C19" s="137" t="s">
+      <c r="C19" s="134" t="s">
         <v>390</v>
       </c>
-      <c r="D19" s="137"/>
+      <c r="D19" s="134"/>
       <c r="E19" s="107"/>
       <c r="F19" s="59" t="s">
         <v>391</v>
@@ -5212,12 +5315,12 @@
     </row>
     <row r="22" spans="2:8" ht="19.5" x14ac:dyDescent="0.35">
       <c r="B22" s="12"/>
-      <c r="C22" s="129" t="s">
+      <c r="C22" s="135" t="s">
         <v>441</v>
       </c>
-      <c r="D22" s="129"/>
-      <c r="E22" s="129"/>
-      <c r="F22" s="129"/>
+      <c r="D22" s="135"/>
+      <c r="E22" s="135"/>
+      <c r="F22" s="135"/>
       <c r="G22" s="12"/>
       <c r="H22" s="108" t="s">
         <v>400</v>
@@ -5231,18 +5334,18 @@
       <c r="D23" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="E23" s="130" t="s">
+      <c r="E23" s="129" t="s">
         <v>495</v>
       </c>
-      <c r="F23" s="130"/>
+      <c r="F23" s="129"/>
       <c r="G23" s="12"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="12"/>
-      <c r="C24" s="131" t="s">
+      <c r="C24" s="130" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="131"/>
+      <c r="D24" s="130"/>
       <c r="E24" s="2" t="s">
         <v>65</v>
       </c>
@@ -5253,10 +5356,10 @@
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="12"/>
-      <c r="C25" s="132" t="s">
+      <c r="C25" s="131" t="s">
         <v>85</v>
       </c>
-      <c r="D25" s="132"/>
+      <c r="D25" s="131"/>
       <c r="E25" s="3" t="s">
         <v>118</v>
       </c>
@@ -5267,10 +5370,10 @@
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="12"/>
-      <c r="C26" s="132" t="s">
+      <c r="C26" s="131" t="s">
         <v>113</v>
       </c>
-      <c r="D26" s="132"/>
+      <c r="D26" s="131"/>
       <c r="E26" s="3" t="s">
         <v>114</v>
       </c>
@@ -5281,10 +5384,10 @@
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" s="12"/>
-      <c r="C27" s="132" t="s">
+      <c r="C27" s="131" t="s">
         <v>184</v>
       </c>
-      <c r="D27" s="132"/>
+      <c r="D27" s="131"/>
       <c r="E27" s="3" t="s">
         <v>185</v>
       </c>
@@ -5295,10 +5398,10 @@
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28" s="12"/>
-      <c r="C28" s="135" t="s">
+      <c r="C28" s="133" t="s">
         <v>183</v>
       </c>
-      <c r="D28" s="135"/>
+      <c r="D28" s="133"/>
       <c r="E28" s="58" t="s">
         <v>182</v>
       </c>
@@ -5309,10 +5412,10 @@
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29" s="12"/>
-      <c r="C29" s="132" t="s">
+      <c r="C29" s="131" t="s">
         <v>86</v>
       </c>
-      <c r="D29" s="132"/>
+      <c r="D29" s="131"/>
       <c r="E29" s="3" t="s">
         <v>127</v>
       </c>
@@ -5323,10 +5426,10 @@
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" s="12"/>
-      <c r="C30" s="132" t="s">
+      <c r="C30" s="131" t="s">
         <v>125</v>
       </c>
-      <c r="D30" s="132"/>
+      <c r="D30" s="131"/>
       <c r="E30" s="3" t="s">
         <v>114</v>
       </c>
@@ -5337,10 +5440,10 @@
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" s="12"/>
-      <c r="C31" s="132" t="s">
+      <c r="C31" s="131" t="s">
         <v>189</v>
       </c>
-      <c r="D31" s="132"/>
+      <c r="D31" s="131"/>
       <c r="E31" s="3" t="s">
         <v>185</v>
       </c>
@@ -5351,10 +5454,10 @@
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B32" s="12"/>
-      <c r="C32" s="135" t="s">
+      <c r="C32" s="133" t="s">
         <v>191</v>
       </c>
-      <c r="D32" s="135"/>
+      <c r="D32" s="133"/>
       <c r="E32" s="58" t="s">
         <v>182</v>
       </c>
@@ -5365,10 +5468,10 @@
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B33" s="12"/>
-      <c r="C33" s="132" t="s">
+      <c r="C33" s="131" t="s">
         <v>87</v>
       </c>
-      <c r="D33" s="132"/>
+      <c r="D33" s="131"/>
       <c r="E33" s="4" t="s">
         <v>136</v>
       </c>
@@ -5379,10 +5482,10 @@
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B34" s="12"/>
-      <c r="C34" s="132" t="s">
+      <c r="C34" s="131" t="s">
         <v>134</v>
       </c>
-      <c r="D34" s="132"/>
+      <c r="D34" s="131"/>
       <c r="E34" s="3" t="s">
         <v>114</v>
       </c>
@@ -5393,10 +5496,10 @@
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B35" s="12"/>
-      <c r="C35" s="132" t="s">
+      <c r="C35" s="131" t="s">
         <v>192</v>
       </c>
-      <c r="D35" s="132"/>
+      <c r="D35" s="131"/>
       <c r="E35" s="3" t="s">
         <v>185</v>
       </c>
@@ -5407,10 +5510,10 @@
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B36" s="12"/>
-      <c r="C36" s="135" t="s">
+      <c r="C36" s="133" t="s">
         <v>193</v>
       </c>
-      <c r="D36" s="135"/>
+      <c r="D36" s="133"/>
       <c r="E36" s="58" t="s">
         <v>182</v>
       </c>
@@ -5421,10 +5524,10 @@
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B37" s="12"/>
-      <c r="C37" s="132" t="s">
+      <c r="C37" s="131" t="s">
         <v>88</v>
       </c>
-      <c r="D37" s="132"/>
+      <c r="D37" s="131"/>
       <c r="E37" s="4" t="s">
         <v>150</v>
       </c>
@@ -5435,10 +5538,10 @@
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B38" s="12"/>
-      <c r="C38" s="132" t="s">
+      <c r="C38" s="131" t="s">
         <v>142</v>
       </c>
-      <c r="D38" s="132"/>
+      <c r="D38" s="131"/>
       <c r="E38" s="4" t="s">
         <v>114</v>
       </c>
@@ -5449,10 +5552,10 @@
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B39" s="12"/>
-      <c r="C39" s="132" t="s">
+      <c r="C39" s="131" t="s">
         <v>195</v>
       </c>
-      <c r="D39" s="132"/>
+      <c r="D39" s="131"/>
       <c r="E39" s="3" t="s">
         <v>185</v>
       </c>
@@ -5463,10 +5566,10 @@
     </row>
     <row r="40" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="12"/>
-      <c r="C40" s="135" t="s">
+      <c r="C40" s="133" t="s">
         <v>196</v>
       </c>
-      <c r="D40" s="135"/>
+      <c r="D40" s="133"/>
       <c r="E40" s="58" t="s">
         <v>182</v>
       </c>
@@ -5477,10 +5580,10 @@
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B41" s="12"/>
-      <c r="C41" s="132" t="s">
+      <c r="C41" s="131" t="s">
         <v>89</v>
       </c>
-      <c r="D41" s="132"/>
+      <c r="D41" s="131"/>
       <c r="E41" s="4" t="s">
         <v>145</v>
       </c>
@@ -5491,10 +5594,10 @@
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B42" s="12"/>
-      <c r="C42" s="132" t="s">
+      <c r="C42" s="131" t="s">
         <v>143</v>
       </c>
-      <c r="D42" s="132"/>
+      <c r="D42" s="131"/>
       <c r="E42" s="3" t="s">
         <v>114</v>
       </c>
@@ -5505,10 +5608,10 @@
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B43" s="12"/>
-      <c r="C43" s="132" t="s">
+      <c r="C43" s="131" t="s">
         <v>202</v>
       </c>
-      <c r="D43" s="132"/>
+      <c r="D43" s="131"/>
       <c r="E43" s="3" t="s">
         <v>185</v>
       </c>
@@ -5519,10 +5622,10 @@
     </row>
     <row r="44" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="12"/>
-      <c r="C44" s="135" t="s">
+      <c r="C44" s="133" t="s">
         <v>203</v>
       </c>
-      <c r="D44" s="135"/>
+      <c r="D44" s="133"/>
       <c r="E44" s="58" t="s">
         <v>182</v>
       </c>
@@ -5533,10 +5636,10 @@
     </row>
     <row r="45" spans="2:7" ht="28.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B45" s="12"/>
-      <c r="C45" s="132" t="s">
+      <c r="C45" s="131" t="s">
         <v>206</v>
       </c>
-      <c r="D45" s="132"/>
+      <c r="D45" s="131"/>
       <c r="E45" s="67" t="s">
         <v>207</v>
       </c>
@@ -5547,10 +5650,10 @@
     </row>
     <row r="46" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B46" s="12"/>
-      <c r="C46" s="133" t="s">
+      <c r="C46" s="132" t="s">
         <v>209</v>
       </c>
-      <c r="D46" s="133"/>
+      <c r="D46" s="132"/>
       <c r="E46" s="73" t="s">
         <v>210</v>
       </c>
@@ -5577,12 +5680,12 @@
     </row>
     <row r="49" spans="2:9" ht="19.5" x14ac:dyDescent="0.35">
       <c r="B49" s="12"/>
-      <c r="C49" s="129" t="s">
+      <c r="C49" s="135" t="s">
         <v>442</v>
       </c>
-      <c r="D49" s="129"/>
-      <c r="E49" s="129"/>
-      <c r="F49" s="129"/>
+      <c r="D49" s="135"/>
+      <c r="E49" s="135"/>
+      <c r="F49" s="135"/>
       <c r="G49" s="12"/>
       <c r="H49" s="108" t="s">
         <v>402</v>
@@ -5596,18 +5699,18 @@
       <c r="D50" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="E50" s="130" t="s">
+      <c r="E50" s="129" t="s">
         <v>493</v>
       </c>
-      <c r="F50" s="130"/>
+      <c r="F50" s="129"/>
       <c r="G50" s="12"/>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B51" s="12"/>
-      <c r="C51" s="131" t="s">
+      <c r="C51" s="130" t="s">
         <v>64</v>
       </c>
-      <c r="D51" s="131"/>
+      <c r="D51" s="130"/>
       <c r="E51" s="45" t="s">
         <v>65</v>
       </c>
@@ -5618,10 +5721,10 @@
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B52" s="12"/>
-      <c r="C52" s="130" t="s">
+      <c r="C52" s="129" t="s">
         <v>280</v>
       </c>
-      <c r="D52" s="130"/>
+      <c r="D52" s="129"/>
       <c r="E52" s="3" t="s">
         <v>465</v>
       </c>
@@ -5632,10 +5735,10 @@
     </row>
     <row r="53" spans="2:9" ht="27.75" x14ac:dyDescent="0.3">
       <c r="B53" s="12"/>
-      <c r="C53" s="132" t="s">
+      <c r="C53" s="131" t="s">
         <v>281</v>
       </c>
-      <c r="D53" s="132"/>
+      <c r="D53" s="131"/>
       <c r="E53" s="3" t="s">
         <v>466</v>
       </c>
@@ -5646,10 +5749,10 @@
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B54" s="12"/>
-      <c r="C54" s="135" t="s">
+      <c r="C54" s="133" t="s">
         <v>285</v>
       </c>
-      <c r="D54" s="135"/>
+      <c r="D54" s="133"/>
       <c r="E54" s="58" t="s">
         <v>467</v>
       </c>
@@ -5661,10 +5764,10 @@
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B55" s="12"/>
-      <c r="C55" s="132" t="s">
+      <c r="C55" s="131" t="s">
         <v>282</v>
       </c>
-      <c r="D55" s="132"/>
+      <c r="D55" s="131"/>
       <c r="E55" s="3" t="s">
         <v>468</v>
       </c>
@@ -5675,10 +5778,10 @@
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B56" s="12"/>
-      <c r="C56" s="135" t="s">
+      <c r="C56" s="133" t="s">
         <v>286</v>
       </c>
-      <c r="D56" s="135"/>
+      <c r="D56" s="133"/>
       <c r="E56" s="58" t="s">
         <v>469</v>
       </c>
@@ -5690,10 +5793,10 @@
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B57" s="12"/>
-      <c r="C57" s="132" t="s">
+      <c r="C57" s="131" t="s">
         <v>283</v>
       </c>
-      <c r="D57" s="132"/>
+      <c r="D57" s="131"/>
       <c r="E57" s="3" t="s">
         <v>470</v>
       </c>
@@ -5704,10 +5807,10 @@
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B58" s="12"/>
-      <c r="C58" s="135" t="s">
+      <c r="C58" s="133" t="s">
         <v>287</v>
       </c>
-      <c r="D58" s="135"/>
+      <c r="D58" s="133"/>
       <c r="E58" s="58" t="s">
         <v>471</v>
       </c>
@@ -5718,10 +5821,10 @@
     </row>
     <row r="59" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="12"/>
-      <c r="C59" s="136" t="s">
+      <c r="C59" s="137" t="s">
         <v>300</v>
       </c>
-      <c r="D59" s="136"/>
+      <c r="D59" s="137"/>
       <c r="E59" s="3" t="s">
         <v>472</v>
       </c>
@@ -5732,10 +5835,10 @@
     </row>
     <row r="60" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="12"/>
-      <c r="C60" s="132" t="s">
+      <c r="C60" s="131" t="s">
         <v>284</v>
       </c>
-      <c r="D60" s="132"/>
+      <c r="D60" s="131"/>
       <c r="E60" s="3" t="s">
         <v>473</v>
       </c>
@@ -5746,10 +5849,10 @@
     </row>
     <row r="61" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="12"/>
-      <c r="C61" s="135" t="s">
+      <c r="C61" s="133" t="s">
         <v>298</v>
       </c>
-      <c r="D61" s="135"/>
+      <c r="D61" s="133"/>
       <c r="E61" s="58" t="s">
         <v>474</v>
       </c>
@@ -5760,10 +5863,10 @@
     </row>
     <row r="62" spans="2:9" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B62" s="12"/>
-      <c r="C62" s="132" t="s">
+      <c r="C62" s="131" t="s">
         <v>292</v>
       </c>
-      <c r="D62" s="132"/>
+      <c r="D62" s="131"/>
       <c r="E62" s="116" t="s">
         <v>490</v>
       </c>
@@ -5774,10 +5877,10 @@
     </row>
     <row r="63" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B63" s="12"/>
-      <c r="C63" s="133" t="s">
+      <c r="C63" s="132" t="s">
         <v>314</v>
       </c>
-      <c r="D63" s="133"/>
+      <c r="D63" s="132"/>
       <c r="E63" s="73" t="s">
         <v>475</v>
       </c>
@@ -5788,10 +5891,10 @@
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B64" s="12"/>
-      <c r="C64" s="134" t="s">
+      <c r="C64" s="136" t="s">
         <v>302</v>
       </c>
-      <c r="D64" s="134"/>
+      <c r="D64" s="136"/>
       <c r="E64" s="69"/>
       <c r="F64" s="70" t="s">
         <v>313</v>
@@ -5816,12 +5919,12 @@
     </row>
     <row r="67" spans="2:8" ht="19.5" x14ac:dyDescent="0.35">
       <c r="B67" s="12"/>
-      <c r="C67" s="129" t="s">
+      <c r="C67" s="135" t="s">
         <v>443</v>
       </c>
-      <c r="D67" s="129"/>
-      <c r="E67" s="129"/>
-      <c r="F67" s="129"/>
+      <c r="D67" s="135"/>
+      <c r="E67" s="135"/>
+      <c r="F67" s="135"/>
       <c r="G67" s="12"/>
       <c r="H67" s="108" t="s">
         <v>404</v>
@@ -5835,18 +5938,18 @@
       <c r="D68" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="E68" s="130" t="s">
+      <c r="E68" s="129" t="s">
         <v>496</v>
       </c>
-      <c r="F68" s="130"/>
+      <c r="F68" s="129"/>
       <c r="G68" s="12"/>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B69" s="12"/>
-      <c r="C69" s="131" t="s">
+      <c r="C69" s="130" t="s">
         <v>64</v>
       </c>
-      <c r="D69" s="131"/>
+      <c r="D69" s="130"/>
       <c r="E69" s="45" t="s">
         <v>65</v>
       </c>
@@ -5857,10 +5960,10 @@
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B70" s="12"/>
-      <c r="C70" s="130" t="s">
+      <c r="C70" s="129" t="s">
         <v>338</v>
       </c>
-      <c r="D70" s="130"/>
+      <c r="D70" s="129"/>
       <c r="E70" s="3" t="s">
         <v>476</v>
       </c>
@@ -5871,10 +5974,10 @@
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B71" s="12"/>
-      <c r="C71" s="135" t="s">
+      <c r="C71" s="133" t="s">
         <v>339</v>
       </c>
-      <c r="D71" s="135"/>
+      <c r="D71" s="133"/>
       <c r="E71" s="58" t="s">
         <v>179</v>
       </c>
@@ -5885,10 +5988,10 @@
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B72" s="12"/>
-      <c r="C72" s="130" t="s">
+      <c r="C72" s="129" t="s">
         <v>336</v>
       </c>
-      <c r="D72" s="130"/>
+      <c r="D72" s="129"/>
       <c r="E72" s="3" t="s">
         <v>477</v>
       </c>
@@ -5899,10 +6002,10 @@
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B73" s="12"/>
-      <c r="C73" s="135" t="s">
+      <c r="C73" s="133" t="s">
         <v>337</v>
       </c>
-      <c r="D73" s="135"/>
+      <c r="D73" s="133"/>
       <c r="E73" s="58" t="s">
         <v>179</v>
       </c>
@@ -5913,10 +6016,10 @@
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B74" s="12"/>
-      <c r="C74" s="132" t="s">
+      <c r="C74" s="131" t="s">
         <v>343</v>
       </c>
-      <c r="D74" s="132"/>
+      <c r="D74" s="131"/>
       <c r="E74" s="3" t="s">
         <v>478</v>
       </c>
@@ -5927,10 +6030,10 @@
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B75" s="12"/>
-      <c r="C75" s="135" t="s">
+      <c r="C75" s="133" t="s">
         <v>344</v>
       </c>
-      <c r="D75" s="135"/>
+      <c r="D75" s="133"/>
       <c r="E75" s="58" t="s">
         <v>479</v>
       </c>
@@ -5941,10 +6044,10 @@
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B76" s="12"/>
-      <c r="C76" s="136" t="s">
+      <c r="C76" s="137" t="s">
         <v>347</v>
       </c>
-      <c r="D76" s="136"/>
+      <c r="D76" s="137"/>
       <c r="E76" s="3" t="s">
         <v>480</v>
       </c>
@@ -5955,10 +6058,10 @@
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B77" s="12"/>
-      <c r="C77" s="132" t="s">
+      <c r="C77" s="131" t="s">
         <v>348</v>
       </c>
-      <c r="D77" s="132"/>
+      <c r="D77" s="131"/>
       <c r="E77" s="3" t="s">
         <v>481</v>
       </c>
@@ -5969,10 +6072,10 @@
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B78" s="12"/>
-      <c r="C78" s="135" t="s">
+      <c r="C78" s="133" t="s">
         <v>298</v>
       </c>
-      <c r="D78" s="135"/>
+      <c r="D78" s="133"/>
       <c r="E78" s="58" t="s">
         <v>467</v>
       </c>
@@ -5983,10 +6086,10 @@
     </row>
     <row r="79" spans="2:8" ht="55.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B79" s="12"/>
-      <c r="C79" s="132" t="s">
+      <c r="C79" s="131" t="s">
         <v>292</v>
       </c>
-      <c r="D79" s="132"/>
+      <c r="D79" s="131"/>
       <c r="E79" s="116" t="s">
         <v>491</v>
       </c>
@@ -5997,10 +6100,10 @@
     </row>
     <row r="80" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B80" s="12"/>
-      <c r="C80" s="133" t="s">
+      <c r="C80" s="132" t="s">
         <v>350</v>
       </c>
-      <c r="D80" s="133"/>
+      <c r="D80" s="132"/>
       <c r="E80" s="73" t="s">
         <v>482</v>
       </c>
@@ -6011,10 +6114,10 @@
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B81" s="12"/>
-      <c r="C81" s="134" t="s">
+      <c r="C81" s="136" t="s">
         <v>302</v>
       </c>
-      <c r="D81" s="134"/>
+      <c r="D81" s="136"/>
       <c r="E81" s="69"/>
       <c r="F81" s="70" t="s">
         <v>351</v>
@@ -6039,12 +6142,12 @@
     </row>
     <row r="84" spans="2:8" ht="19.5" x14ac:dyDescent="0.35">
       <c r="B84" s="12"/>
-      <c r="C84" s="129" t="s">
+      <c r="C84" s="135" t="s">
         <v>444</v>
       </c>
-      <c r="D84" s="129"/>
-      <c r="E84" s="129"/>
-      <c r="F84" s="129"/>
+      <c r="D84" s="135"/>
+      <c r="E84" s="135"/>
+      <c r="F84" s="135"/>
       <c r="G84" s="12"/>
       <c r="H84" s="108" t="s">
         <v>406</v>
@@ -6058,18 +6161,18 @@
       <c r="D85" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="E85" s="130" t="s">
+      <c r="E85" s="129" t="s">
         <v>502</v>
       </c>
-      <c r="F85" s="130"/>
+      <c r="F85" s="129"/>
       <c r="G85" s="12"/>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B86" s="12"/>
-      <c r="C86" s="131" t="s">
+      <c r="C86" s="130" t="s">
         <v>64</v>
       </c>
-      <c r="D86" s="131"/>
+      <c r="D86" s="130"/>
       <c r="E86" s="45" t="s">
         <v>65</v>
       </c>
@@ -6080,10 +6183,10 @@
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B87" s="12"/>
-      <c r="C87" s="130" t="s">
+      <c r="C87" s="129" t="s">
         <v>364</v>
       </c>
-      <c r="D87" s="130"/>
+      <c r="D87" s="129"/>
       <c r="E87" s="3" t="s">
         <v>483</v>
       </c>
@@ -6094,10 +6197,10 @@
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B88" s="12"/>
-      <c r="C88" s="135" t="s">
+      <c r="C88" s="133" t="s">
         <v>376</v>
       </c>
-      <c r="D88" s="135"/>
+      <c r="D88" s="133"/>
       <c r="E88" s="58" t="s">
         <v>479</v>
       </c>
@@ -6108,10 +6211,10 @@
     </row>
     <row r="89" spans="2:8" ht="27.75" x14ac:dyDescent="0.3">
       <c r="B89" s="12"/>
-      <c r="C89" s="130" t="s">
+      <c r="C89" s="129" t="s">
         <v>366</v>
       </c>
-      <c r="D89" s="130"/>
+      <c r="D89" s="129"/>
       <c r="E89" s="3" t="s">
         <v>484</v>
       </c>
@@ -6122,10 +6225,10 @@
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B90" s="12"/>
-      <c r="C90" s="135" t="s">
+      <c r="C90" s="133" t="s">
         <v>367</v>
       </c>
-      <c r="D90" s="135"/>
+      <c r="D90" s="133"/>
       <c r="E90" s="58" t="s">
         <v>474</v>
       </c>
@@ -6136,10 +6239,10 @@
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B91" s="12"/>
-      <c r="C91" s="132" t="s">
+      <c r="C91" s="131" t="s">
         <v>369</v>
       </c>
-      <c r="D91" s="132"/>
+      <c r="D91" s="131"/>
       <c r="E91" s="3" t="s">
         <v>485</v>
       </c>
@@ -6150,10 +6253,10 @@
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B92" s="12"/>
-      <c r="C92" s="135" t="s">
+      <c r="C92" s="133" t="s">
         <v>370</v>
       </c>
-      <c r="D92" s="135"/>
+      <c r="D92" s="133"/>
       <c r="E92" s="58" t="s">
         <v>486</v>
       </c>
@@ -6164,10 +6267,10 @@
     </row>
     <row r="93" spans="2:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B93" s="12"/>
-      <c r="C93" s="132" t="s">
+      <c r="C93" s="131" t="s">
         <v>292</v>
       </c>
-      <c r="D93" s="132"/>
+      <c r="D93" s="131"/>
       <c r="E93" s="116" t="s">
         <v>492</v>
       </c>
@@ -6178,10 +6281,10 @@
     </row>
     <row r="94" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B94" s="12"/>
-      <c r="C94" s="133" t="s">
+      <c r="C94" s="132" t="s">
         <v>374</v>
       </c>
-      <c r="D94" s="133"/>
+      <c r="D94" s="132"/>
       <c r="E94" s="73" t="s">
         <v>487</v>
       </c>
@@ -6192,10 +6295,10 @@
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B95" s="12"/>
-      <c r="C95" s="134" t="s">
+      <c r="C95" s="136" t="s">
         <v>302</v>
       </c>
-      <c r="D95" s="134"/>
+      <c r="D95" s="136"/>
       <c r="E95" s="69"/>
       <c r="F95" s="70" t="s">
         <v>375</v>
@@ -6212,20 +6315,58 @@
     </row>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C84:F84"/>
+    <mergeCell ref="E85:F85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C81:D81"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C75:D75"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C67:F67"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="C69:D69"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C59:D59"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C49:F49"/>
     <mergeCell ref="E50:F50"/>
@@ -6242,58 +6383,20 @@
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="C38:D38"/>
     <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C67:F67"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C84:F84"/>
-    <mergeCell ref="E85:F85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C39:D39"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H11" location="'Set NonZero Values'!A1" display="'Set NonZero Values'!A1"/>
@@ -6344,10 +6447,10 @@
     </row>
     <row r="6" spans="2:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="12"/>
-      <c r="D6" s="144" t="s">
+      <c r="D6" s="147" t="s">
         <v>504</v>
       </c>
-      <c r="E6" s="145"/>
+      <c r="E6" s="148"/>
       <c r="F6" s="12"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
@@ -6358,10 +6461,10 @@
     </row>
     <row r="8" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C8" s="12"/>
-      <c r="D8" s="138" t="s">
+      <c r="D8" s="141" t="s">
         <v>420</v>
       </c>
-      <c r="E8" s="139"/>
+      <c r="E8" s="142"/>
       <c r="F8" s="12"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
@@ -6444,10 +6547,10 @@
     </row>
     <row r="18" spans="3:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C18" s="12"/>
-      <c r="D18" s="138" t="s">
+      <c r="D18" s="141" t="s">
         <v>386</v>
       </c>
-      <c r="E18" s="139"/>
+      <c r="E18" s="142"/>
       <c r="F18" s="12"/>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.3">
@@ -6553,11 +6656,11 @@
     </row>
     <row r="6" spans="2:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B6" s="17"/>
-      <c r="C6" s="152" t="s">
+      <c r="C6" s="155" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="152"/>
-      <c r="E6" s="152"/>
+      <c r="D6" s="155"/>
+      <c r="E6" s="155"/>
       <c r="F6" s="17"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
@@ -6659,11 +6762,11 @@
     </row>
     <row r="16" spans="2:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B16" s="17"/>
-      <c r="C16" s="129" t="s">
+      <c r="C16" s="135" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="153"/>
-      <c r="E16" s="153"/>
+      <c r="D16" s="156"/>
+      <c r="E16" s="156"/>
       <c r="F16" s="17"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
@@ -6815,11 +6918,11 @@
     </row>
     <row r="29" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B29" s="17"/>
-      <c r="C29" s="129" t="s">
+      <c r="C29" s="135" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="153"/>
-      <c r="E29" s="153"/>
+      <c r="D29" s="156"/>
+      <c r="E29" s="156"/>
       <c r="F29" s="17"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.3">
@@ -7438,12 +7541,12 @@
     </row>
     <row r="6" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B6" s="17"/>
-      <c r="C6" s="157" t="s">
+      <c r="C6" s="160" t="s">
         <v>105</v>
       </c>
-      <c r="D6" s="157"/>
-      <c r="E6" s="157"/>
-      <c r="F6" s="157"/>
+      <c r="D6" s="160"/>
+      <c r="E6" s="160"/>
+      <c r="F6" s="160"/>
       <c r="G6" s="28"/>
       <c r="H6" s="48"/>
       <c r="I6" s="48"/>
@@ -7569,11 +7672,11 @@
     <row r="16" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
-      <c r="D16" s="152" t="s">
+      <c r="D16" s="155" t="s">
         <v>106</v>
       </c>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
+      <c r="E16" s="157"/>
+      <c r="F16" s="157"/>
       <c r="G16" s="28"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
@@ -7747,11 +7850,11 @@
     <row r="30" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
-      <c r="D30" s="155" t="s">
+      <c r="D30" s="158" t="s">
         <v>107</v>
       </c>
-      <c r="E30" s="154"/>
-      <c r="F30" s="156"/>
+      <c r="E30" s="157"/>
+      <c r="F30" s="159"/>
       <c r="G30" s="28"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.3">
@@ -8085,12 +8188,12 @@
     </row>
     <row r="6" spans="2:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B6" s="12"/>
-      <c r="C6" s="129" t="s">
+      <c r="C6" s="135" t="s">
         <v>439</v>
       </c>
-      <c r="D6" s="129"/>
-      <c r="E6" s="129"/>
-      <c r="F6" s="129"/>
+      <c r="D6" s="135"/>
+      <c r="E6" s="135"/>
+      <c r="F6" s="135"/>
       <c r="G6" s="12"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
@@ -8297,10 +8400,10 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="12"/>
-      <c r="C6" s="138" t="s">
+      <c r="C6" s="141" t="s">
         <v>438</v>
       </c>
-      <c r="D6" s="139"/>
+      <c r="D6" s="142"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
     </row>
@@ -8362,11 +8465,11 @@
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="12"/>
-      <c r="C13" s="140" t="s">
+      <c r="C13" s="143" t="s">
         <v>445</v>
       </c>
-      <c r="D13" s="141"/>
-      <c r="E13" s="141"/>
+      <c r="D13" s="144"/>
+      <c r="E13" s="144"/>
       <c r="F13" s="12"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
@@ -8433,10 +8536,10 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="12"/>
-      <c r="C20" s="142" t="s">
+      <c r="C20" s="145" t="s">
         <v>446</v>
       </c>
-      <c r="D20" s="142"/>
+      <c r="D20" s="145"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
     </row>
@@ -8498,10 +8601,10 @@
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="12"/>
-      <c r="C27" s="142" t="s">
+      <c r="C27" s="145" t="s">
         <v>447</v>
       </c>
-      <c r="D27" s="142"/>
+      <c r="D27" s="145"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
     </row>
@@ -8563,10 +8666,10 @@
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" s="12"/>
-      <c r="C34" s="142" t="s">
+      <c r="C34" s="145" t="s">
         <v>448</v>
       </c>
-      <c r="D34" s="142"/>
+      <c r="D34" s="145"/>
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
     </row>
@@ -8637,9 +8740,11 @@
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B1:H83"/>
+  <dimension ref="B1:H91"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="E88" sqref="E88"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
@@ -8673,10 +8778,10 @@
     <row r="6" spans="2:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
-      <c r="D6" s="144" t="s">
+      <c r="D6" s="147" t="s">
         <v>503</v>
       </c>
-      <c r="E6" s="145"/>
+      <c r="E6" s="148"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
     </row>
@@ -8699,10 +8804,10 @@
     <row r="9" spans="2:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
-      <c r="D9" s="138" t="s">
+      <c r="D9" s="141" t="s">
         <v>505</v>
       </c>
-      <c r="E9" s="139"/>
+      <c r="E9" s="142"/>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
     </row>
@@ -8785,10 +8890,10 @@
     <row r="17" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
-      <c r="D17" s="138" t="s">
+      <c r="D17" s="141" t="s">
         <v>506</v>
       </c>
-      <c r="E17" s="139"/>
+      <c r="E17" s="142"/>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
     </row>
@@ -8871,10 +8976,10 @@
     <row r="25" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
-      <c r="D25" s="138" t="s">
+      <c r="D25" s="141" t="s">
         <v>507</v>
       </c>
-      <c r="E25" s="139"/>
+      <c r="E25" s="142"/>
       <c r="F25" s="12"/>
       <c r="G25" s="12"/>
     </row>
@@ -8956,12 +9061,12 @@
     </row>
     <row r="33" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B33" s="12"/>
-      <c r="C33" s="138" t="s">
+      <c r="C33" s="141" t="s">
         <v>260</v>
       </c>
-      <c r="D33" s="138"/>
-      <c r="E33" s="138"/>
-      <c r="F33" s="138"/>
+      <c r="D33" s="141"/>
+      <c r="E33" s="141"/>
+      <c r="F33" s="141"/>
       <c r="G33" s="12"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.3">
@@ -9025,7 +9130,7 @@
       <c r="C38" s="46">
         <v>1</v>
       </c>
-      <c r="D38" s="130" t="s">
+      <c r="D38" s="129" t="s">
         <v>28</v>
       </c>
       <c r="E38" s="46" t="s">
@@ -9041,7 +9146,7 @@
       <c r="C39" s="46">
         <v>2</v>
       </c>
-      <c r="D39" s="130"/>
+      <c r="D39" s="129"/>
       <c r="E39" s="46" t="s">
         <v>164</v>
       </c>
@@ -9055,7 +9160,7 @@
       <c r="C40" s="46">
         <v>3</v>
       </c>
-      <c r="D40" s="130"/>
+      <c r="D40" s="129"/>
       <c r="E40" s="46" t="s">
         <v>165</v>
       </c>
@@ -9069,7 +9174,7 @@
       <c r="C41" s="60">
         <v>4</v>
       </c>
-      <c r="D41" s="143"/>
+      <c r="D41" s="146"/>
       <c r="E41" s="60" t="s">
         <v>166</v>
       </c>
@@ -9083,7 +9188,7 @@
       <c r="C42" s="63">
         <v>5</v>
       </c>
-      <c r="D42" s="146" t="s">
+      <c r="D42" s="149" t="s">
         <v>157</v>
       </c>
       <c r="E42" s="63" t="s">
@@ -9099,7 +9204,7 @@
       <c r="C43" s="46">
         <v>6</v>
       </c>
-      <c r="D43" s="130"/>
+      <c r="D43" s="129"/>
       <c r="E43" s="46" t="s">
         <v>170</v>
       </c>
@@ -9113,7 +9218,7 @@
       <c r="C44" s="46">
         <v>7</v>
       </c>
-      <c r="D44" s="130"/>
+      <c r="D44" s="129"/>
       <c r="E44" s="46" t="s">
         <v>171</v>
       </c>
@@ -9127,7 +9232,7 @@
       <c r="C45" s="60">
         <v>8</v>
       </c>
-      <c r="D45" s="143"/>
+      <c r="D45" s="146"/>
       <c r="E45" s="60" t="s">
         <v>172</v>
       </c>
@@ -9141,7 +9246,7 @@
       <c r="C46" s="63">
         <v>9</v>
       </c>
-      <c r="D46" s="146" t="s">
+      <c r="D46" s="149" t="s">
         <v>23</v>
       </c>
       <c r="E46" s="63" t="s">
@@ -9157,7 +9262,7 @@
       <c r="C47" s="46">
         <v>10</v>
       </c>
-      <c r="D47" s="130"/>
+      <c r="D47" s="129"/>
       <c r="E47" s="46" t="s">
         <v>131</v>
       </c>
@@ -9171,7 +9276,7 @@
       <c r="C48" s="46">
         <v>11</v>
       </c>
-      <c r="D48" s="130"/>
+      <c r="D48" s="129"/>
       <c r="E48" s="46" t="s">
         <v>132</v>
       </c>
@@ -9185,7 +9290,7 @@
       <c r="C49" s="60">
         <v>12</v>
       </c>
-      <c r="D49" s="143"/>
+      <c r="D49" s="146"/>
       <c r="E49" s="60" t="s">
         <v>133</v>
       </c>
@@ -9199,7 +9304,7 @@
       <c r="C50" s="46">
         <v>13</v>
       </c>
-      <c r="D50" s="130" t="s">
+      <c r="D50" s="129" t="s">
         <v>162</v>
       </c>
       <c r="E50" s="46" t="s">
@@ -9215,7 +9320,7 @@
       <c r="C51" s="46">
         <v>14</v>
       </c>
-      <c r="D51" s="130"/>
+      <c r="D51" s="129"/>
       <c r="E51" s="46" t="s">
         <v>173</v>
       </c>
@@ -9229,7 +9334,7 @@
       <c r="C52" s="46">
         <v>15</v>
       </c>
-      <c r="D52" s="130"/>
+      <c r="D52" s="129"/>
       <c r="E52" s="46" t="s">
         <v>168</v>
       </c>
@@ -9243,7 +9348,7 @@
       <c r="C53" s="60">
         <v>16</v>
       </c>
-      <c r="D53" s="143"/>
+      <c r="D53" s="146"/>
       <c r="E53" s="60" t="s">
         <v>169</v>
       </c>
@@ -9257,7 +9362,7 @@
       <c r="C54" s="46">
         <v>13</v>
       </c>
-      <c r="D54" s="130"/>
+      <c r="D54" s="129"/>
       <c r="E54" s="46" t="s">
         <v>159</v>
       </c>
@@ -9271,7 +9376,7 @@
       <c r="C55" s="46">
         <v>14</v>
       </c>
-      <c r="D55" s="130"/>
+      <c r="D55" s="129"/>
       <c r="E55" s="46" t="s">
         <v>167</v>
       </c>
@@ -9285,7 +9390,7 @@
       <c r="C56" s="46">
         <v>15</v>
       </c>
-      <c r="D56" s="130"/>
+      <c r="D56" s="129"/>
       <c r="E56" s="46" t="s">
         <v>174</v>
       </c>
@@ -9299,7 +9404,7 @@
       <c r="C57" s="60">
         <v>16</v>
       </c>
-      <c r="D57" s="143"/>
+      <c r="D57" s="146"/>
       <c r="E57" s="60" t="s">
         <v>175</v>
       </c>
@@ -9327,10 +9432,10 @@
     <row r="60" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B60" s="12"/>
       <c r="C60" s="12"/>
-      <c r="D60" s="138" t="s">
+      <c r="D60" s="141" t="s">
         <v>508</v>
       </c>
-      <c r="E60" s="139"/>
+      <c r="E60" s="142"/>
       <c r="F60" s="12"/>
       <c r="G60" s="12"/>
     </row>
@@ -9413,10 +9518,10 @@
     <row r="68" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B68" s="12"/>
       <c r="C68" s="12"/>
-      <c r="D68" s="138" t="s">
+      <c r="D68" s="141" t="s">
         <v>188</v>
       </c>
-      <c r="E68" s="139"/>
+      <c r="E68" s="142"/>
       <c r="F68" s="12"/>
       <c r="G68" s="12"/>
     </row>
@@ -9511,10 +9616,10 @@
     <row r="77" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B77" s="12"/>
       <c r="C77" s="12"/>
-      <c r="D77" s="138" t="s">
+      <c r="D77" s="141" t="s">
         <v>509</v>
       </c>
-      <c r="E77" s="139"/>
+      <c r="E77" s="142"/>
       <c r="F77" s="12"/>
       <c r="G77" s="12"/>
     </row>
@@ -9586,8 +9691,95 @@
       <c r="F83" s="12"/>
       <c r="G83" s="12"/>
     </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B84" s="12"/>
+      <c r="C84" s="12"/>
+      <c r="D84" s="12"/>
+      <c r="E84" s="12"/>
+      <c r="F84" s="12"/>
+      <c r="G84" s="12"/>
+    </row>
+    <row r="85" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B85" s="12"/>
+      <c r="C85" s="12"/>
+      <c r="D85" s="141" t="s">
+        <v>517</v>
+      </c>
+      <c r="E85" s="142"/>
+      <c r="F85" s="12"/>
+      <c r="G85" s="12"/>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B86" s="12"/>
+      <c r="C86" s="12"/>
+      <c r="D86" s="51" t="s">
+        <v>176</v>
+      </c>
+      <c r="E86" s="52" t="s">
+        <v>177</v>
+      </c>
+      <c r="F86" s="12"/>
+      <c r="G86" s="12"/>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B87" s="12"/>
+      <c r="C87" s="12"/>
+      <c r="D87" s="126" t="s">
+        <v>118</v>
+      </c>
+      <c r="E87" s="65">
+        <v>0.11120764499999999</v>
+      </c>
+      <c r="F87" s="12"/>
+      <c r="G87" s="12"/>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B88" s="12"/>
+      <c r="C88" s="12"/>
+      <c r="D88" s="126" t="s">
+        <v>127</v>
+      </c>
+      <c r="E88" s="65">
+        <v>5.4117651000000003E-2</v>
+      </c>
+      <c r="F88" s="12"/>
+      <c r="G88" s="12"/>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B89" s="12"/>
+      <c r="C89" s="12"/>
+      <c r="D89" s="126" t="s">
+        <v>136</v>
+      </c>
+      <c r="E89" s="65">
+        <v>0.42000000100000001</v>
+      </c>
+      <c r="F89" s="12"/>
+      <c r="G89" s="12"/>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B90" s="12"/>
+      <c r="C90" s="12"/>
+      <c r="D90" s="61" t="s">
+        <v>145</v>
+      </c>
+      <c r="E90" s="66">
+        <v>0.41467470299999998</v>
+      </c>
+      <c r="F90" s="12"/>
+      <c r="G90" s="12"/>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B91" s="12"/>
+      <c r="C91" s="12"/>
+      <c r="D91" s="12"/>
+      <c r="E91" s="12"/>
+      <c r="F91" s="12"/>
+      <c r="G91" s="12"/>
+    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
+    <mergeCell ref="D85:E85"/>
     <mergeCell ref="D50:D53"/>
     <mergeCell ref="D68:E68"/>
     <mergeCell ref="D77:E77"/>
@@ -9658,10 +9850,10 @@
     </row>
     <row r="6" spans="2:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="12"/>
-      <c r="C6" s="144" t="s">
+      <c r="C6" s="147" t="s">
         <v>497</v>
       </c>
-      <c r="D6" s="145"/>
+      <c r="D6" s="148"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -9682,10 +9874,10 @@
     </row>
     <row r="8" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B8" s="12"/>
-      <c r="C8" s="138" t="s">
+      <c r="C8" s="141" t="s">
         <v>234</v>
       </c>
-      <c r="D8" s="139"/>
+      <c r="D8" s="142"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
@@ -9713,7 +9905,7 @@
       <c r="C10" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="151">
+      <c r="D10" s="152">
         <v>3</v>
       </c>
       <c r="E10" s="12"/>
@@ -9728,7 +9920,7 @@
       <c r="C11" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="151"/>
+      <c r="D11" s="152"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
@@ -9741,7 +9933,7 @@
       <c r="C12" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="150"/>
+      <c r="D12" s="151"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
       <c r="G12" s="12"/>
@@ -9786,12 +9978,12 @@
     </row>
     <row r="16" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B16" s="12"/>
-      <c r="C16" s="138" t="s">
+      <c r="C16" s="141" t="s">
         <v>510</v>
       </c>
-      <c r="D16" s="138"/>
-      <c r="E16" s="138"/>
-      <c r="F16" s="138"/>
+      <c r="D16" s="141"/>
+      <c r="E16" s="141"/>
+      <c r="F16" s="141"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
@@ -9822,10 +10014,10 @@
         <v>239</v>
       </c>
       <c r="D18" s="46"/>
-      <c r="E18" s="130" t="s">
+      <c r="E18" s="129" t="s">
         <v>243</v>
       </c>
-      <c r="F18" s="149">
+      <c r="F18" s="150">
         <v>3</v>
       </c>
       <c r="G18" s="12"/>
@@ -9839,8 +10031,8 @@
       <c r="D19" s="60" t="s">
         <v>247</v>
       </c>
-      <c r="E19" s="143"/>
-      <c r="F19" s="149"/>
+      <c r="E19" s="146"/>
+      <c r="F19" s="150"/>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
@@ -9852,10 +10044,10 @@
         <v>240</v>
       </c>
       <c r="D20" s="63"/>
-      <c r="E20" s="146" t="s">
+      <c r="E20" s="149" t="s">
         <v>245</v>
       </c>
-      <c r="F20" s="149"/>
+      <c r="F20" s="150"/>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
@@ -9867,8 +10059,8 @@
       <c r="D21" s="60" t="s">
         <v>248</v>
       </c>
-      <c r="E21" s="143"/>
-      <c r="F21" s="149"/>
+      <c r="E21" s="146"/>
+      <c r="F21" s="150"/>
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
@@ -9880,10 +10072,10 @@
         <v>241</v>
       </c>
       <c r="D22" s="46"/>
-      <c r="E22" s="130" t="s">
+      <c r="E22" s="129" t="s">
         <v>246</v>
       </c>
-      <c r="F22" s="149"/>
+      <c r="F22" s="150"/>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
@@ -9895,8 +10087,8 @@
       <c r="D23" s="60" t="s">
         <v>242</v>
       </c>
-      <c r="E23" s="143"/>
-      <c r="F23" s="150"/>
+      <c r="E23" s="146"/>
+      <c r="F23" s="151"/>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
@@ -9939,10 +10131,10 @@
     </row>
     <row r="27" spans="2:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B27" s="12"/>
-      <c r="C27" s="138" t="s">
+      <c r="C27" s="141" t="s">
         <v>257</v>
       </c>
-      <c r="D27" s="139"/>
+      <c r="D27" s="142"/>
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
@@ -10019,10 +10211,10 @@
     </row>
     <row r="33" spans="2:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B33" s="12"/>
-      <c r="C33" s="138" t="s">
+      <c r="C33" s="141" t="s">
         <v>254</v>
       </c>
-      <c r="D33" s="139"/>
+      <c r="D33" s="142"/>
       <c r="E33" s="12"/>
       <c r="F33" s="12"/>
       <c r="G33" s="12"/>
@@ -10114,15 +10306,15 @@
     </row>
     <row r="40" spans="2:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B40" s="12"/>
-      <c r="C40" s="138" t="s">
+      <c r="C40" s="141" t="s">
         <v>301</v>
       </c>
-      <c r="D40" s="138"/>
-      <c r="E40" s="138"/>
-      <c r="F40" s="138"/>
-      <c r="G40" s="138"/>
-      <c r="H40" s="138"/>
-      <c r="I40" s="138"/>
+      <c r="D40" s="141"/>
+      <c r="E40" s="141"/>
+      <c r="F40" s="141"/>
+      <c r="G40" s="141"/>
+      <c r="H40" s="141"/>
+      <c r="I40" s="141"/>
       <c r="J40" s="12"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.3">
@@ -10136,12 +10328,12 @@
       <c r="E41" s="78" t="s">
         <v>263</v>
       </c>
-      <c r="F41" s="147" t="s">
+      <c r="F41" s="153" t="s">
         <v>264</v>
       </c>
-      <c r="G41" s="147"/>
-      <c r="H41" s="147"/>
-      <c r="I41" s="147"/>
+      <c r="G41" s="153"/>
+      <c r="H41" s="153"/>
+      <c r="I41" s="153"/>
       <c r="J41" s="12"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.3">
@@ -10155,12 +10347,12 @@
       <c r="E42" s="86" t="s">
         <v>263</v>
       </c>
-      <c r="F42" s="148" t="s">
+      <c r="F42" s="154" t="s">
         <v>273</v>
       </c>
-      <c r="G42" s="148"/>
-      <c r="H42" s="148"/>
-      <c r="I42" s="148"/>
+      <c r="G42" s="154"/>
+      <c r="H42" s="154"/>
+      <c r="I42" s="154"/>
       <c r="J42" s="12"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.3">
@@ -10309,10 +10501,10 @@
     </row>
     <row r="51" spans="2:10" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B51" s="12"/>
-      <c r="C51" s="138" t="s">
+      <c r="C51" s="141" t="s">
         <v>276</v>
       </c>
-      <c r="D51" s="139"/>
+      <c r="D51" s="142"/>
       <c r="E51" s="12"/>
       <c r="F51" s="12"/>
       <c r="G51" s="12"/>
@@ -10378,6 +10570,11 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C40:I40"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F18:F23"/>
@@ -10387,11 +10584,6 @@
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="D10:D12"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C40:I40"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K1" location="'Rating Algorithm'!A48" display="'Rating Algorithm'!A48"/>
@@ -10405,10 +10597,10 @@
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="B3:G21"/>
+  <dimension ref="B3:G36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:D16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -10416,6 +10608,7 @@
     <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.77734375" style="79" customWidth="1"/>
     <col min="5" max="5" width="17.5546875" style="79" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -10435,12 +10628,12 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="12"/>
-      <c r="C6" s="142" t="s">
+      <c r="C6" s="145" t="s">
         <v>450</v>
       </c>
-      <c r="D6" s="142"/>
-      <c r="E6" s="142"/>
-      <c r="F6" s="142"/>
+      <c r="D6" s="145"/>
+      <c r="E6" s="145"/>
+      <c r="F6" s="145"/>
       <c r="G6" s="12"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
@@ -10573,10 +10766,10 @@
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" s="12"/>
-      <c r="C16" s="142" t="s">
+      <c r="C16" s="145" t="s">
         <v>449</v>
       </c>
-      <c r="D16" s="142"/>
+      <c r="D16" s="145"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
@@ -10635,12 +10828,177 @@
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
     </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+    </row>
+    <row r="23" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="135" t="s">
+        <v>521</v>
+      </c>
+      <c r="E23" s="135"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="161" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="85" t="s">
+        <v>518</v>
+      </c>
+      <c r="F24" s="12">
+        <v>5</v>
+      </c>
+      <c r="G24" s="12"/>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="161" t="s">
+        <v>519</v>
+      </c>
+      <c r="E25" s="85" t="s">
+        <v>224</v>
+      </c>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="51" t="s">
+        <v>176</v>
+      </c>
+      <c r="E26" s="52" t="s">
+        <v>177</v>
+      </c>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="126" t="s">
+        <v>118</v>
+      </c>
+      <c r="E27" s="65">
+        <v>0.11121358000000001</v>
+      </c>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="61" t="s">
+        <v>127</v>
+      </c>
+      <c r="E28" s="66">
+        <v>5.4100910000000002E-2</v>
+      </c>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+    </row>
+    <row r="31" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="135" t="s">
+        <v>522</v>
+      </c>
+      <c r="E31" s="135"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="161" t="s">
+        <v>519</v>
+      </c>
+      <c r="E32" s="85" t="s">
+        <v>520</v>
+      </c>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="51" t="s">
+        <v>176</v>
+      </c>
+      <c r="E33" s="52" t="s">
+        <v>177</v>
+      </c>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="126" t="s">
+        <v>136</v>
+      </c>
+      <c r="E34" s="65">
+        <v>0.42</v>
+      </c>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="61" t="s">
+        <v>145</v>
+      </c>
+      <c r="E35" s="66">
+        <v>0.41</v>
+      </c>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="C16:D16"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D31:E31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10690,10 +11048,10 @@
     </row>
     <row r="6" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="12"/>
-      <c r="C6" s="144" t="s">
+      <c r="C6" s="147" t="s">
         <v>498</v>
       </c>
-      <c r="D6" s="145"/>
+      <c r="D6" s="148"/>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -10722,10 +11080,10 @@
     </row>
     <row r="8" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B8" s="12"/>
-      <c r="C8" s="138" t="s">
+      <c r="C8" s="141" t="s">
         <v>316</v>
       </c>
-      <c r="D8" s="139"/>
+      <c r="D8" s="142"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
@@ -10826,10 +11184,10 @@
     </row>
     <row r="14" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B14" s="12"/>
-      <c r="C14" s="138" t="s">
+      <c r="C14" s="141" t="s">
         <v>321</v>
       </c>
-      <c r="D14" s="139"/>
+      <c r="D14" s="142"/>
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
@@ -10949,10 +11307,10 @@
     </row>
     <row r="21" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B21" s="12"/>
-      <c r="C21" s="138" t="s">
+      <c r="C21" s="141" t="s">
         <v>322</v>
       </c>
-      <c r="D21" s="139"/>
+      <c r="D21" s="142"/>
       <c r="E21" s="12"/>
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
@@ -11072,19 +11430,19 @@
     </row>
     <row r="28" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B28" s="12"/>
-      <c r="C28" s="138" t="s">
+      <c r="C28" s="141" t="s">
         <v>326</v>
       </c>
-      <c r="D28" s="138"/>
-      <c r="E28" s="138"/>
-      <c r="F28" s="138"/>
-      <c r="G28" s="138"/>
-      <c r="H28" s="138"/>
-      <c r="I28" s="138"/>
-      <c r="J28" s="138"/>
-      <c r="K28" s="138"/>
-      <c r="L28" s="138"/>
-      <c r="M28" s="138"/>
+      <c r="D28" s="141"/>
+      <c r="E28" s="141"/>
+      <c r="F28" s="141"/>
+      <c r="G28" s="141"/>
+      <c r="H28" s="141"/>
+      <c r="I28" s="141"/>
+      <c r="J28" s="141"/>
+      <c r="K28" s="141"/>
+      <c r="L28" s="141"/>
+      <c r="M28" s="141"/>
       <c r="N28" s="12"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.3">
@@ -11098,16 +11456,16 @@
       <c r="E29" s="78" t="s">
         <v>263</v>
       </c>
-      <c r="F29" s="147" t="s">
+      <c r="F29" s="153" t="s">
         <v>264</v>
       </c>
-      <c r="G29" s="147"/>
-      <c r="H29" s="147"/>
-      <c r="I29" s="147"/>
-      <c r="J29" s="147"/>
-      <c r="K29" s="147"/>
-      <c r="L29" s="147"/>
-      <c r="M29" s="147"/>
+      <c r="G29" s="153"/>
+      <c r="H29" s="153"/>
+      <c r="I29" s="153"/>
+      <c r="J29" s="153"/>
+      <c r="K29" s="153"/>
+      <c r="L29" s="153"/>
+      <c r="M29" s="153"/>
       <c r="N29" s="12"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.3">
@@ -11121,16 +11479,16 @@
       <c r="E30" s="86" t="s">
         <v>263</v>
       </c>
-      <c r="F30" s="148" t="s">
+      <c r="F30" s="154" t="s">
         <v>328</v>
       </c>
-      <c r="G30" s="148"/>
-      <c r="H30" s="148"/>
-      <c r="I30" s="148"/>
-      <c r="J30" s="148"/>
-      <c r="K30" s="148"/>
-      <c r="L30" s="148"/>
-      <c r="M30" s="148"/>
+      <c r="G30" s="154"/>
+      <c r="H30" s="154"/>
+      <c r="I30" s="154"/>
+      <c r="J30" s="154"/>
+      <c r="K30" s="154"/>
+      <c r="L30" s="154"/>
+      <c r="M30" s="154"/>
       <c r="N30" s="12"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.3">
@@ -11427,11 +11785,11 @@
     </row>
     <row r="43" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B43" s="12"/>
-      <c r="C43" s="138" t="s">
+      <c r="C43" s="141" t="s">
         <v>333</v>
       </c>
-      <c r="D43" s="138"/>
-      <c r="E43" s="138"/>
+      <c r="D43" s="141"/>
+      <c r="E43" s="141"/>
       <c r="F43" s="12"/>
       <c r="G43" s="12"/>
       <c r="H43" s="12"/>
@@ -11469,7 +11827,7 @@
         <v>11</v>
       </c>
       <c r="D45" s="46"/>
-      <c r="E45" s="149" t="s">
+      <c r="E45" s="150" t="s">
         <v>279</v>
       </c>
       <c r="F45" s="12"/>
@@ -11488,7 +11846,7 @@
       <c r="D46" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="E46" s="150"/>
+      <c r="E46" s="151"/>
       <c r="F46" s="12"/>
       <c r="G46" s="12"/>
       <c r="H46" s="12"/>
@@ -11533,6 +11891,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="E45:E46"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C14:D14"/>
@@ -11540,8 +11900,6 @@
     <mergeCell ref="F30:M30"/>
     <mergeCell ref="F29:M29"/>
     <mergeCell ref="C28:M28"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="E45:E46"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="O1" location="'Rating Algorithm'!A66" display="'Rating Algorithm'!A66"/>
@@ -11582,10 +11940,10 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" s="12"/>
-      <c r="C6" s="142" t="s">
+      <c r="C6" s="145" t="s">
         <v>451</v>
       </c>
-      <c r="D6" s="142"/>
+      <c r="D6" s="145"/>
       <c r="E6" s="12"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
@@ -11652,10 +12010,10 @@
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" s="12"/>
-      <c r="C14" s="142" t="s">
+      <c r="C14" s="145" t="s">
         <v>452</v>
       </c>
-      <c r="D14" s="142"/>
+      <c r="D14" s="145"/>
       <c r="E14" s="12"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
@@ -11746,10 +12104,10 @@
     </row>
     <row r="6" spans="2:6" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="12"/>
-      <c r="C6" s="144" t="s">
+      <c r="C6" s="147" t="s">
         <v>499</v>
       </c>
-      <c r="D6" s="145"/>
+      <c r="D6" s="148"/>
       <c r="E6" s="12"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
@@ -11760,10 +12118,10 @@
     </row>
     <row r="8" spans="2:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B8" s="12"/>
-      <c r="C8" s="138" t="s">
+      <c r="C8" s="141" t="s">
         <v>355</v>
       </c>
-      <c r="D8" s="139"/>
+      <c r="D8" s="142"/>
       <c r="E8" s="12"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
@@ -11810,10 +12168,10 @@
     </row>
     <row r="14" spans="2:6" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B14" s="12"/>
-      <c r="C14" s="138" t="s">
+      <c r="C14" s="141" t="s">
         <v>358</v>
       </c>
-      <c r="D14" s="139"/>
+      <c r="D14" s="142"/>
       <c r="E14" s="12"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
@@ -11860,10 +12218,10 @@
     </row>
     <row r="20" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B20" s="12"/>
-      <c r="C20" s="138" t="s">
+      <c r="C20" s="141" t="s">
         <v>361</v>
       </c>
-      <c r="D20" s="139"/>
+      <c r="D20" s="142"/>
       <c r="E20" s="12"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
@@ -11923,7 +12281,7 @@
   </sheetPr>
   <dimension ref="B1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
@@ -11958,12 +12316,12 @@
     </row>
     <row r="6" spans="2:9" ht="124.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="12"/>
-      <c r="D6" s="144" t="s">
+      <c r="D6" s="147" t="s">
         <v>500</v>
       </c>
-      <c r="E6" s="144"/>
-      <c r="F6" s="144"/>
-      <c r="G6" s="144"/>
+      <c r="E6" s="147"/>
+      <c r="F6" s="147"/>
+      <c r="G6" s="147"/>
       <c r="H6" s="12"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
@@ -11976,10 +12334,10 @@
     </row>
     <row r="8" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C8" s="12"/>
-      <c r="D8" s="138" t="s">
+      <c r="D8" s="141" t="s">
         <v>511</v>
       </c>
-      <c r="E8" s="139"/>
+      <c r="E8" s="142"/>
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
@@ -12066,20 +12424,20 @@
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C17" s="12"/>
-      <c r="D17" s="152" t="s">
+      <c r="D17" s="155" t="s">
         <v>514</v>
       </c>
-      <c r="E17" s="152"/>
+      <c r="E17" s="155"/>
       <c r="F17" s="12"/>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
     </row>
     <row r="18" spans="3:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C18" s="12"/>
-      <c r="D18" s="138" t="s">
+      <c r="D18" s="141" t="s">
         <v>453</v>
       </c>
-      <c r="E18" s="138"/>
+      <c r="E18" s="141"/>
       <c r="F18" s="12" t="s">
         <v>515</v>
       </c>
@@ -12176,20 +12534,20 @@
     </row>
     <row r="27" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C27" s="12"/>
-      <c r="D27" s="152" t="s">
+      <c r="D27" s="155" t="s">
         <v>516</v>
       </c>
-      <c r="E27" s="152"/>
+      <c r="E27" s="155"/>
       <c r="F27" s="12"/>
       <c r="G27" s="12"/>
       <c r="H27" s="12"/>
     </row>
     <row r="28" spans="3:8" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C28" s="12"/>
-      <c r="D28" s="138" t="s">
+      <c r="D28" s="141" t="s">
         <v>453</v>
       </c>
-      <c r="E28" s="138"/>
+      <c r="E28" s="141"/>
       <c r="F28" s="12" t="s">
         <v>515</v>
       </c>
@@ -12201,7 +12559,7 @@
       <c r="D29" s="83" t="s">
         <v>354</v>
       </c>
-      <c r="E29" s="159" t="s">
+      <c r="E29" s="128" t="s">
         <v>384</v>
       </c>
       <c r="F29" s="12"/>
@@ -12334,12 +12692,12 @@
     </row>
     <row r="43" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C43" s="12"/>
-      <c r="D43" s="152" t="s">
+      <c r="D43" s="155" t="s">
         <v>513</v>
       </c>
-      <c r="E43" s="152"/>
-      <c r="F43" s="152"/>
-      <c r="G43" s="152"/>
+      <c r="E43" s="155"/>
+      <c r="F43" s="155"/>
+      <c r="G43" s="155"/>
       <c r="H43" s="12"/>
     </row>
     <row r="44" spans="3:8" x14ac:dyDescent="0.3">
@@ -12353,7 +12711,7 @@
       <c r="F44" s="125" t="s">
         <v>266</v>
       </c>
-      <c r="G44" s="158" t="s">
+      <c r="G44" s="127" t="s">
         <v>307</v>
       </c>
       <c r="H44" s="12"/>
@@ -12720,13 +13078,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D6:G6"/>
     <mergeCell ref="D43:G43"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I1" location="'Rating Algorithm'!A16" display="'Rating Algorithm'!A16"/>

</xml_diff>